<commit_message>
MOSIP-15883_added template codes (#633)
</commit_message>
<xml_diff>
--- a/data-dml/mosip_master/dml/master-template.xlsx
+++ b/data-dml/mosip_master/dml/master-template.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A39FC0-212B-4239-918A-BBA397E11B31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4377" uniqueCount="823">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4557" uniqueCount="847">
   <si>
     <t>id</t>
   </si>
@@ -2501,12 +2500,84 @@
   <si>
     <t>Cher $!name_fra,
 Votre demande d'UIN pour l'ID d'enregistrement : $!RID est en attente car vous avez besoin de détails supplémentaires avec AdditionalInfoRequestId $!additionalInfoRequestId et additionalInfoProcess $!additionalInfoProcess. Veuillez visiter votre bureau d'enregistrement le plus proche ou visitez https://mosip.io/grievances pour progresser sur l'application de l'UIN.</t>
+  </si>
+  <si>
+    <t>Registration Failed because you have already Registered</t>
+  </si>
+  <si>
+    <t>RPR_DUP_UIN_EMAIL_SUB</t>
+  </si>
+  <si>
+    <t>L'inscription a échoué car vous êtes déjà inscrit</t>
+  </si>
+  <si>
+    <t>فشل التسجيل لأنك قمت بالتسجيل بالفعل</t>
+  </si>
+  <si>
+    <t>Re-Register because there was a Technical Issue</t>
+  </si>
+  <si>
+    <t>Réinscrivez-vous car il y a eu un problème technique</t>
+  </si>
+  <si>
+    <t>إعادة التسجيل بسبب وجود مشكلة فنية</t>
+  </si>
+  <si>
+    <t>RPR_TEC_ISSUE_EMAIL_SUB</t>
+  </si>
+  <si>
+    <t>RPR_UIN_REAC_EMAIL_SUB</t>
+  </si>
+  <si>
+    <t>RPR_UIN_DEAC_EMAIL_SUB</t>
+  </si>
+  <si>
+    <t>RPR_UIN_GEN_EMAIL_SUB</t>
+  </si>
+  <si>
+    <t>RPR_UIN_UPD_EMAIL_SUB</t>
+  </si>
+  <si>
+    <t>Uin is activated successfully</t>
+  </si>
+  <si>
+    <t>تم تفعيل Uin بنجاح</t>
+  </si>
+  <si>
+    <t>Uin est activé avec succès</t>
+  </si>
+  <si>
+    <t>Uin is deactivated</t>
+  </si>
+  <si>
+    <t>Uin est désactivé</t>
+  </si>
+  <si>
+    <t>تم إلغاء تنشيط Uin</t>
+  </si>
+  <si>
+    <t>UIN Generated</t>
+  </si>
+  <si>
+    <t>تم إنشاء UIN</t>
+  </si>
+  <si>
+    <t>UIN généré</t>
+  </si>
+  <si>
+    <t>UIN Details Updated</t>
+  </si>
+  <si>
+    <t>تم تحديث تفاصيل UIN</t>
+  </si>
+  <si>
+    <t>Détails UIN mis à jour</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2820,11 +2891,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M437"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M455"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A436" workbookViewId="0">
-      <selection activeCell="F438" sqref="F438"/>
+    <sheetView tabSelected="1" topLeftCell="A438" workbookViewId="0">
+      <selection activeCell="F456" sqref="F456"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20752,8 +20823,746 @@
         <v>20</v>
       </c>
     </row>
+    <row r="438" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A438">
+        <v>1274</v>
+      </c>
+      <c r="B438" t="s">
+        <v>823</v>
+      </c>
+      <c r="C438" t="s">
+        <v>823</v>
+      </c>
+      <c r="D438" t="s">
+        <v>14</v>
+      </c>
+      <c r="E438" t="s">
+        <v>28</v>
+      </c>
+      <c r="F438" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="G438">
+        <v>10003</v>
+      </c>
+      <c r="H438" t="s">
+        <v>46</v>
+      </c>
+      <c r="I438" t="s">
+        <v>824</v>
+      </c>
+      <c r="J438" t="s">
+        <v>18</v>
+      </c>
+      <c r="K438" t="b">
+        <v>1</v>
+      </c>
+      <c r="L438" t="s">
+        <v>19</v>
+      </c>
+      <c r="M438" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="439" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A439">
+        <v>1274</v>
+      </c>
+      <c r="B439" t="s">
+        <v>825</v>
+      </c>
+      <c r="C439" t="s">
+        <v>825</v>
+      </c>
+      <c r="D439" t="s">
+        <v>14</v>
+      </c>
+      <c r="E439" t="s">
+        <v>28</v>
+      </c>
+      <c r="F439" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="G439">
+        <v>10003</v>
+      </c>
+      <c r="H439" t="s">
+        <v>46</v>
+      </c>
+      <c r="I439" t="s">
+        <v>824</v>
+      </c>
+      <c r="J439" t="s">
+        <v>39</v>
+      </c>
+      <c r="K439" t="b">
+        <v>1</v>
+      </c>
+      <c r="L439" t="s">
+        <v>19</v>
+      </c>
+      <c r="M439" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="440" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A440">
+        <v>1274</v>
+      </c>
+      <c r="B440" t="s">
+        <v>826</v>
+      </c>
+      <c r="C440" t="s">
+        <v>826</v>
+      </c>
+      <c r="D440" t="s">
+        <v>14</v>
+      </c>
+      <c r="E440" t="s">
+        <v>28</v>
+      </c>
+      <c r="F440" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="G440">
+        <v>10003</v>
+      </c>
+      <c r="H440" t="s">
+        <v>46</v>
+      </c>
+      <c r="I440" t="s">
+        <v>824</v>
+      </c>
+      <c r="J440" t="s">
+        <v>31</v>
+      </c>
+      <c r="K440" t="b">
+        <v>1</v>
+      </c>
+      <c r="L440" t="s">
+        <v>19</v>
+      </c>
+      <c r="M440" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="441" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A441">
+        <v>1275</v>
+      </c>
+      <c r="B441" t="s">
+        <v>827</v>
+      </c>
+      <c r="C441" t="s">
+        <v>827</v>
+      </c>
+      <c r="D441" t="s">
+        <v>14</v>
+      </c>
+      <c r="E441" t="s">
+        <v>28</v>
+      </c>
+      <c r="F441" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="G441">
+        <v>10003</v>
+      </c>
+      <c r="H441" t="s">
+        <v>46</v>
+      </c>
+      <c r="I441" t="s">
+        <v>830</v>
+      </c>
+      <c r="J441" t="s">
+        <v>18</v>
+      </c>
+      <c r="K441" t="b">
+        <v>1</v>
+      </c>
+      <c r="L441" t="s">
+        <v>19</v>
+      </c>
+      <c r="M441" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="442" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A442">
+        <v>1275</v>
+      </c>
+      <c r="B442" t="s">
+        <v>828</v>
+      </c>
+      <c r="C442" t="s">
+        <v>828</v>
+      </c>
+      <c r="D442" t="s">
+        <v>14</v>
+      </c>
+      <c r="E442" t="s">
+        <v>28</v>
+      </c>
+      <c r="F442" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="G442">
+        <v>10003</v>
+      </c>
+      <c r="H442" t="s">
+        <v>46</v>
+      </c>
+      <c r="I442" t="s">
+        <v>830</v>
+      </c>
+      <c r="J442" t="s">
+        <v>39</v>
+      </c>
+      <c r="K442" t="b">
+        <v>1</v>
+      </c>
+      <c r="L442" t="s">
+        <v>19</v>
+      </c>
+      <c r="M442" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="443" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A443">
+        <v>1275</v>
+      </c>
+      <c r="B443" t="s">
+        <v>829</v>
+      </c>
+      <c r="C443" t="s">
+        <v>829</v>
+      </c>
+      <c r="D443" t="s">
+        <v>14</v>
+      </c>
+      <c r="E443" t="s">
+        <v>28</v>
+      </c>
+      <c r="F443" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="G443">
+        <v>10003</v>
+      </c>
+      <c r="H443" t="s">
+        <v>46</v>
+      </c>
+      <c r="I443" t="s">
+        <v>830</v>
+      </c>
+      <c r="J443" t="s">
+        <v>31</v>
+      </c>
+      <c r="K443" t="b">
+        <v>1</v>
+      </c>
+      <c r="L443" t="s">
+        <v>19</v>
+      </c>
+      <c r="M443" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="444" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A444">
+        <v>1276</v>
+      </c>
+      <c r="B444" t="s">
+        <v>835</v>
+      </c>
+      <c r="C444" t="s">
+        <v>835</v>
+      </c>
+      <c r="D444" t="s">
+        <v>14</v>
+      </c>
+      <c r="E444" t="s">
+        <v>28</v>
+      </c>
+      <c r="F444" t="s">
+        <v>835</v>
+      </c>
+      <c r="G444">
+        <v>10003</v>
+      </c>
+      <c r="H444" t="s">
+        <v>46</v>
+      </c>
+      <c r="I444" t="s">
+        <v>831</v>
+      </c>
+      <c r="J444" t="s">
+        <v>18</v>
+      </c>
+      <c r="K444" t="b">
+        <v>1</v>
+      </c>
+      <c r="L444" t="s">
+        <v>19</v>
+      </c>
+      <c r="M444" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="445" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A445">
+        <v>1276</v>
+      </c>
+      <c r="B445" t="s">
+        <v>837</v>
+      </c>
+      <c r="C445" t="s">
+        <v>837</v>
+      </c>
+      <c r="D445" t="s">
+        <v>14</v>
+      </c>
+      <c r="E445" t="s">
+        <v>28</v>
+      </c>
+      <c r="F445" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="G445">
+        <v>10003</v>
+      </c>
+      <c r="H445" t="s">
+        <v>46</v>
+      </c>
+      <c r="I445" t="s">
+        <v>831</v>
+      </c>
+      <c r="J445" t="s">
+        <v>39</v>
+      </c>
+      <c r="K445" t="b">
+        <v>1</v>
+      </c>
+      <c r="L445" t="s">
+        <v>19</v>
+      </c>
+      <c r="M445" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="446" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A446">
+        <v>1276</v>
+      </c>
+      <c r="B446" t="s">
+        <v>836</v>
+      </c>
+      <c r="C446" t="s">
+        <v>836</v>
+      </c>
+      <c r="D446" t="s">
+        <v>14</v>
+      </c>
+      <c r="E446" t="s">
+        <v>28</v>
+      </c>
+      <c r="F446" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="G446">
+        <v>10003</v>
+      </c>
+      <c r="H446" t="s">
+        <v>46</v>
+      </c>
+      <c r="I446" t="s">
+        <v>831</v>
+      </c>
+      <c r="J446" t="s">
+        <v>31</v>
+      </c>
+      <c r="K446" t="b">
+        <v>1</v>
+      </c>
+      <c r="L446" t="s">
+        <v>19</v>
+      </c>
+      <c r="M446" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="447" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A447">
+        <v>1277</v>
+      </c>
+      <c r="B447" t="s">
+        <v>838</v>
+      </c>
+      <c r="C447" t="s">
+        <v>838</v>
+      </c>
+      <c r="D447" t="s">
+        <v>14</v>
+      </c>
+      <c r="E447" t="s">
+        <v>28</v>
+      </c>
+      <c r="F447" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="G447">
+        <v>10003</v>
+      </c>
+      <c r="H447" t="s">
+        <v>46</v>
+      </c>
+      <c r="I447" t="s">
+        <v>832</v>
+      </c>
+      <c r="J447" t="s">
+        <v>18</v>
+      </c>
+      <c r="K447" t="b">
+        <v>1</v>
+      </c>
+      <c r="L447" t="s">
+        <v>19</v>
+      </c>
+      <c r="M447" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="448" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A448">
+        <v>1277</v>
+      </c>
+      <c r="B448" t="s">
+        <v>839</v>
+      </c>
+      <c r="C448" t="s">
+        <v>839</v>
+      </c>
+      <c r="D448" t="s">
+        <v>14</v>
+      </c>
+      <c r="E448" t="s">
+        <v>28</v>
+      </c>
+      <c r="F448" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="G448">
+        <v>10003</v>
+      </c>
+      <c r="H448" t="s">
+        <v>46</v>
+      </c>
+      <c r="I448" t="s">
+        <v>832</v>
+      </c>
+      <c r="J448" t="s">
+        <v>39</v>
+      </c>
+      <c r="K448" t="b">
+        <v>1</v>
+      </c>
+      <c r="L448" t="s">
+        <v>19</v>
+      </c>
+      <c r="M448" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="449" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A449">
+        <v>1277</v>
+      </c>
+      <c r="B449" t="s">
+        <v>840</v>
+      </c>
+      <c r="C449" t="s">
+        <v>840</v>
+      </c>
+      <c r="D449" t="s">
+        <v>14</v>
+      </c>
+      <c r="E449" t="s">
+        <v>28</v>
+      </c>
+      <c r="F449" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="G449">
+        <v>10003</v>
+      </c>
+      <c r="H449" t="s">
+        <v>46</v>
+      </c>
+      <c r="I449" t="s">
+        <v>832</v>
+      </c>
+      <c r="J449" t="s">
+        <v>31</v>
+      </c>
+      <c r="K449" t="b">
+        <v>1</v>
+      </c>
+      <c r="L449" t="s">
+        <v>19</v>
+      </c>
+      <c r="M449" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="450" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A450">
+        <v>1278</v>
+      </c>
+      <c r="B450" t="s">
+        <v>841</v>
+      </c>
+      <c r="C450" t="s">
+        <v>841</v>
+      </c>
+      <c r="D450" t="s">
+        <v>14</v>
+      </c>
+      <c r="E450" t="s">
+        <v>28</v>
+      </c>
+      <c r="F450" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="G450">
+        <v>10003</v>
+      </c>
+      <c r="H450" t="s">
+        <v>46</v>
+      </c>
+      <c r="I450" t="s">
+        <v>833</v>
+      </c>
+      <c r="J450" t="s">
+        <v>18</v>
+      </c>
+      <c r="K450" t="b">
+        <v>1</v>
+      </c>
+      <c r="L450" t="s">
+        <v>19</v>
+      </c>
+      <c r="M450" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="451" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A451">
+        <v>1278</v>
+      </c>
+      <c r="B451" t="s">
+        <v>843</v>
+      </c>
+      <c r="C451" t="s">
+        <v>843</v>
+      </c>
+      <c r="D451" t="s">
+        <v>14</v>
+      </c>
+      <c r="E451" t="s">
+        <v>28</v>
+      </c>
+      <c r="F451" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="G451">
+        <v>10003</v>
+      </c>
+      <c r="H451" t="s">
+        <v>46</v>
+      </c>
+      <c r="I451" t="s">
+        <v>833</v>
+      </c>
+      <c r="J451" t="s">
+        <v>39</v>
+      </c>
+      <c r="K451" t="b">
+        <v>1</v>
+      </c>
+      <c r="L451" t="s">
+        <v>19</v>
+      </c>
+      <c r="M451" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="452" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A452">
+        <v>1278</v>
+      </c>
+      <c r="B452" t="s">
+        <v>842</v>
+      </c>
+      <c r="C452" t="s">
+        <v>842</v>
+      </c>
+      <c r="D452" t="s">
+        <v>14</v>
+      </c>
+      <c r="E452" t="s">
+        <v>28</v>
+      </c>
+      <c r="F452" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="G452">
+        <v>10003</v>
+      </c>
+      <c r="H452" t="s">
+        <v>46</v>
+      </c>
+      <c r="I452" t="s">
+        <v>833</v>
+      </c>
+      <c r="J452" t="s">
+        <v>31</v>
+      </c>
+      <c r="K452" t="b">
+        <v>1</v>
+      </c>
+      <c r="L452" t="s">
+        <v>19</v>
+      </c>
+      <c r="M452" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="453" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A453">
+        <v>1279</v>
+      </c>
+      <c r="B453" t="s">
+        <v>844</v>
+      </c>
+      <c r="C453" t="s">
+        <v>844</v>
+      </c>
+      <c r="D453" t="s">
+        <v>14</v>
+      </c>
+      <c r="E453" t="s">
+        <v>28</v>
+      </c>
+      <c r="F453" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="G453">
+        <v>10003</v>
+      </c>
+      <c r="H453" t="s">
+        <v>46</v>
+      </c>
+      <c r="I453" t="s">
+        <v>834</v>
+      </c>
+      <c r="J453" t="s">
+        <v>18</v>
+      </c>
+      <c r="K453" t="b">
+        <v>1</v>
+      </c>
+      <c r="L453" t="s">
+        <v>19</v>
+      </c>
+      <c r="M453" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="454" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A454">
+        <v>1279</v>
+      </c>
+      <c r="B454" t="s">
+        <v>846</v>
+      </c>
+      <c r="C454" t="s">
+        <v>846</v>
+      </c>
+      <c r="D454" t="s">
+        <v>14</v>
+      </c>
+      <c r="E454" t="s">
+        <v>28</v>
+      </c>
+      <c r="F454" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="G454">
+        <v>10003</v>
+      </c>
+      <c r="H454" t="s">
+        <v>46</v>
+      </c>
+      <c r="I454" t="s">
+        <v>834</v>
+      </c>
+      <c r="J454" t="s">
+        <v>39</v>
+      </c>
+      <c r="K454" t="b">
+        <v>1</v>
+      </c>
+      <c r="L454" t="s">
+        <v>19</v>
+      </c>
+      <c r="M454" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="455" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A455">
+        <v>1279</v>
+      </c>
+      <c r="B455" t="s">
+        <v>845</v>
+      </c>
+      <c r="C455" t="s">
+        <v>845</v>
+      </c>
+      <c r="D455" t="s">
+        <v>14</v>
+      </c>
+      <c r="E455" t="s">
+        <v>28</v>
+      </c>
+      <c r="F455" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="G455">
+        <v>10003</v>
+      </c>
+      <c r="H455" t="s">
+        <v>46</v>
+      </c>
+      <c r="I455" t="s">
+        <v>834</v>
+      </c>
+      <c r="J455" t="s">
+        <v>31</v>
+      </c>
+      <c r="K455" t="b">
+        <v>1</v>
+      </c>
+      <c r="L455" t="s">
+        <v>19</v>
+      </c>
+      <c r="M455" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M1" xr:uid="{493D9055-CB8A-4896-BD32-23224F84A471}"/>
+  <autoFilter ref="A1:M1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>